<commit_message>
added images to icons
</commit_message>
<xml_diff>
--- a/src/data/database.xlsx
+++ b/src/data/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Desktop\USB BackUp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\DABAD\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2DFFA59-A0B3-4603-AF28-50483758B6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15318393-D04A-4925-9291-13C5CEF427FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -792,9 +792,6 @@
     <t>Ratatouille</t>
   </si>
   <si>
-    <t>Monster University</t>
-  </si>
-  <si>
     <t>Dan Scanion</t>
   </si>
   <si>
@@ -1279,6 +1276,9 @@
   </si>
   <si>
     <t>Sam Mendes</t>
+  </si>
+  <si>
+    <t>Monsters University</t>
   </si>
 </sst>
 </file>
@@ -1409,7 +1409,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1461,7 +1461,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1666,8 +1666,8 @@
   <dimension ref="A1:G242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1712,7 +1712,7 @@
         <v>2019</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1734,13 +1734,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C4" s="5">
         <v>2018</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1748,13 +1748,13 @@
         <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C5" s="5">
         <v>2019</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1762,7 +1762,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C6" s="5">
         <v>1988</v>
@@ -1787,13 +1787,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C8" s="5">
         <v>2018</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1815,13 +1815,13 @@
         <v>50</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C10" s="5">
         <v>2009</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1843,13 +1843,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C12" s="5">
         <v>1973</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1913,13 +1913,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C17" s="5">
         <v>2007</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1927,13 +1927,13 @@
         <v>7</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C18" s="5">
         <v>1970</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1983,13 +1983,13 @@
         <v>7</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C22" s="5">
         <v>2019</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2011,13 +2011,13 @@
         <v>7</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C24" s="5">
         <v>2005</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -2039,13 +2039,13 @@
         <v>7</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C26" s="5">
         <v>2006</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2067,7 +2067,7 @@
         <v>7</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C28" s="5">
         <v>2018</v>
@@ -2081,13 +2081,13 @@
         <v>7</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C29" s="5">
         <v>2013</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2095,13 +2095,13 @@
         <v>50</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C30" s="5">
         <v>2004</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2109,13 +2109,13 @@
         <v>7</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C31" s="5">
         <v>1972</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2123,13 +2123,13 @@
         <v>7</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C32" s="5">
         <v>2018</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -2151,13 +2151,13 @@
         <v>7</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C34" s="5">
         <v>2010</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2165,13 +2165,13 @@
         <v>7</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C35" s="5">
         <v>2013</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -2179,7 +2179,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C36" s="5">
         <v>2010</v>
@@ -2193,13 +2193,13 @@
         <v>7</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C37" s="5">
         <v>2012</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -2207,13 +2207,13 @@
         <v>7</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C38" s="5">
         <v>2011</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -2221,13 +2221,13 @@
         <v>7</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C39" s="5">
         <v>2003</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -2249,13 +2249,13 @@
         <v>50</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C41" s="5">
         <v>2008</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -2291,13 +2291,13 @@
         <v>7</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C44" s="5">
         <v>1971</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -2333,7 +2333,7 @@
         <v>50</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C47" s="5">
         <v>2014</v>
@@ -2403,7 +2403,7 @@
         <v>7</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C52" s="5">
         <v>2018</v>
@@ -2417,7 +2417,7 @@
         <v>7</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C53" s="5">
         <v>2018</v>
@@ -2431,13 +2431,13 @@
         <v>7</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C54" s="5">
         <v>2016</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2473,7 +2473,7 @@
         <v>50</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C57" s="5">
         <v>2019</v>
@@ -2501,7 +2501,7 @@
         <v>50</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C59" s="5">
         <v>2019</v>
@@ -2529,13 +2529,13 @@
         <v>7</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C61" s="5">
         <v>1997</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2557,7 +2557,7 @@
         <v>7</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C63" s="5">
         <v>2013</v>
@@ -2571,13 +2571,13 @@
         <v>50</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C64" s="5">
         <v>2016</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2711,13 +2711,13 @@
         <v>50</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C74" s="5">
         <v>2018</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2739,7 +2739,7 @@
         <v>7</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C76" s="5">
         <v>2006</v>
@@ -2750,7 +2750,7 @@
         <v>7</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C77" s="5">
         <v>2007</v>
@@ -2761,7 +2761,7 @@
         <v>7</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C78" s="5">
         <v>2008</v>
@@ -2772,7 +2772,7 @@
         <v>7</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C79" s="5">
         <v>2008</v>
@@ -2783,7 +2783,7 @@
         <v>7</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C80" s="5">
         <v>2010</v>
@@ -2794,7 +2794,7 @@
         <v>7</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C81" s="5">
         <v>2011</v>
@@ -2805,7 +2805,7 @@
         <v>7</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C82" s="5">
         <v>2011</v>
@@ -2816,7 +2816,7 @@
         <v>7</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C83" s="5">
         <v>2012</v>
@@ -2827,13 +2827,13 @@
         <v>7</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C84" s="5">
         <v>2019</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2939,13 +2939,13 @@
         <v>7</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C92" s="5">
         <v>2018</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -2995,7 +2995,7 @@
         <v>7</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C96" s="5">
         <v>2019</v>
@@ -3023,13 +3023,13 @@
         <v>7</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C98" s="5">
         <v>2017</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -3107,7 +3107,7 @@
         <v>7</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C104" s="5">
         <v>2017</v>
@@ -3135,7 +3135,7 @@
         <v>50</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C106" s="5">
         <v>2019</v>
@@ -3149,13 +3149,13 @@
         <v>50</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C107" s="5">
         <v>2017</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -3177,13 +3177,13 @@
         <v>7</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C109" s="5">
         <v>2019</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -3191,13 +3191,13 @@
         <v>50</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C110" s="5">
         <v>2012</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -3205,13 +3205,13 @@
         <v>50</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C111" s="5">
         <v>2016</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -3247,7 +3247,7 @@
         <v>7</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C114" s="5">
         <v>2018</v>
@@ -3261,7 +3261,7 @@
         <v>7</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C115" s="5">
         <v>2015</v>
@@ -3275,13 +3275,13 @@
         <v>7</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C116" s="5">
         <v>2015</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -3331,13 +3331,13 @@
         <v>7</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C120" s="5">
         <v>2018</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -3345,13 +3345,13 @@
         <v>7</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C121" s="5">
         <v>2015</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -3373,13 +3373,13 @@
         <v>7</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>254</v>
+        <v>416</v>
       </c>
       <c r="C123" s="5">
         <v>2013</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -3387,13 +3387,13 @@
         <v>7</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C124" s="5">
         <v>2018</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -3507,13 +3507,13 @@
         <v>50</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C133" s="5">
         <v>2013</v>
       </c>
       <c r="D133" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
@@ -3549,13 +3549,13 @@
         <v>7</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C136" s="5">
         <v>2018</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -3563,13 +3563,13 @@
         <v>7</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C137" s="5">
         <v>2019</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -3619,13 +3619,13 @@
         <v>7</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C141" s="5">
         <v>2018</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
@@ -3675,13 +3675,13 @@
         <v>7</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C145" s="5">
         <v>1968</v>
       </c>
       <c r="D145" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
@@ -3717,7 +3717,7 @@
         <v>7</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C148" s="5">
         <v>2008</v>
@@ -3801,13 +3801,13 @@
         <v>50</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C154" s="5">
         <v>2011</v>
       </c>
       <c r="D154" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
@@ -3843,13 +3843,13 @@
         <v>7</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C157" s="5">
         <v>2004</v>
       </c>
       <c r="D157" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
@@ -3871,13 +3871,13 @@
         <v>7</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C159" s="5">
         <v>2016</v>
       </c>
       <c r="D159" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
@@ -3885,13 +3885,13 @@
         <v>7</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C160" s="5">
         <v>1992</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
@@ -3899,13 +3899,13 @@
         <v>7</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C161" s="5">
         <v>1993</v>
       </c>
       <c r="D161" s="9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
@@ -3913,13 +3913,13 @@
         <v>7</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C162" s="5">
         <v>2012</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
@@ -3927,13 +3927,13 @@
         <v>7</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C163" s="5">
         <v>2015</v>
       </c>
       <c r="D163" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
@@ -3997,13 +3997,13 @@
         <v>7</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C168" s="5">
         <v>2018</v>
       </c>
       <c r="D168" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
@@ -4081,13 +4081,13 @@
         <v>7</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C174" s="5">
         <v>2017</v>
       </c>
       <c r="D174" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
@@ -4095,13 +4095,13 @@
         <v>7</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C175" s="5">
         <v>2016</v>
       </c>
       <c r="D175" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
@@ -4109,13 +4109,13 @@
         <v>7</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C176" s="5">
         <v>1941</v>
       </c>
       <c r="D176" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
@@ -4123,7 +4123,7 @@
         <v>7</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C177" s="5">
         <v>2015</v>
@@ -4221,7 +4221,7 @@
         <v>50</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C184" s="5">
         <v>2014</v>
@@ -4235,13 +4235,13 @@
         <v>7</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C185" s="5">
         <v>2019</v>
       </c>
       <c r="D185" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
@@ -4249,13 +4249,13 @@
         <v>7</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C186" s="5">
         <v>2018</v>
       </c>
       <c r="D186" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.3">
@@ -4263,13 +4263,13 @@
         <v>50</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C187" s="5">
         <v>2010</v>
       </c>
       <c r="D187" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.3">
@@ -4277,7 +4277,7 @@
         <v>7</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C188" s="5">
         <v>2018</v>
@@ -4305,13 +4305,13 @@
         <v>50</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C190" s="5">
         <v>2014</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
@@ -4347,13 +4347,13 @@
         <v>7</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C193" s="5">
         <v>2002</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.3">
@@ -4361,13 +4361,13 @@
         <v>7</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C194" s="5">
         <v>2018</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.3">
@@ -4473,13 +4473,13 @@
         <v>50</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C202" s="5">
         <v>2010</v>
       </c>
       <c r="D202" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.3">
@@ -4557,13 +4557,13 @@
         <v>50</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C208" s="5">
         <v>2018</v>
       </c>
       <c r="D208" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.3">
@@ -4571,13 +4571,13 @@
         <v>7</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C209" s="5">
         <v>2017</v>
       </c>
       <c r="D209" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
@@ -4585,13 +4585,13 @@
         <v>7</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C210" s="5">
         <v>2007</v>
       </c>
       <c r="D210" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
@@ -4613,13 +4613,13 @@
         <v>7</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C212" s="5">
         <v>2004</v>
       </c>
       <c r="D212" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.3">
@@ -4697,13 +4697,13 @@
         <v>7</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C218" s="5">
         <v>2016</v>
       </c>
       <c r="D218" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.3">
@@ -4711,13 +4711,13 @@
         <v>7</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C219" s="5">
         <v>2010</v>
       </c>
       <c r="D219" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.3">
@@ -4753,7 +4753,7 @@
         <v>7</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C222" s="5">
         <v>2019</v>
@@ -4767,7 +4767,7 @@
         <v>7</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C223" s="5">
         <v>2018</v>
@@ -4781,13 +4781,13 @@
         <v>7</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C224" s="5">
         <v>2018</v>
       </c>
       <c r="D224" s="9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
@@ -4865,13 +4865,13 @@
         <v>7</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C230" s="5">
         <v>2018</v>
       </c>
       <c r="D230" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="231" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -4879,13 +4879,13 @@
         <v>50</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C231" s="5">
         <v>2018</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
@@ -4893,13 +4893,13 @@
         <v>7</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C232" s="5">
         <v>2017</v>
       </c>
       <c r="D232" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
@@ -5019,7 +5019,7 @@
         <v>50</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C241" s="5">
         <v>2019</v>
@@ -5048,8 +5048,8 @@
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G268">
-    <sortCondition ref="D1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H242">
+    <sortCondition ref="H1:H242"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update with trolls 2 sing 2 ticket to paradise
</commit_message>
<xml_diff>
--- a/src/data/database.xlsx
+++ b/src/data/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\DABAD\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4219F8-D270-42F4-8224-D43EF1EDF6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14CF6A2-A014-4C2C-9ECD-04ED258BED16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="616">
   <si>
     <t>Title</t>
   </si>
@@ -1861,6 +1861,21 @@
   </si>
   <si>
     <t>Mike Bartlett</t>
+  </si>
+  <si>
+    <t>Sing 2</t>
+  </si>
+  <si>
+    <t>Trolls World Tour</t>
+  </si>
+  <si>
+    <t>Walt Dohrn, David P. Smith</t>
+  </si>
+  <si>
+    <t>Ticket to Paradise</t>
+  </si>
+  <si>
+    <t>Ol Parker</t>
   </si>
 </sst>
 </file>
@@ -2251,11 +2266,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L362"/>
+  <dimension ref="A1:L365"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E363" sqref="E363"/>
+      <pane ySplit="1" topLeftCell="A339" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I365" sqref="I365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8511,7 +8526,7 @@
         <v>422</v>
       </c>
       <c r="H228" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I228" s="10">
         <v>104</v>
@@ -8525,22 +8540,25 @@
         <v>7</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>432</v>
+        <v>611</v>
       </c>
       <c r="D229" s="5">
-        <v>1952</v>
+        <v>2021</v>
       </c>
       <c r="E229" s="9" t="s">
-        <v>434</v>
+        <v>265</v>
       </c>
       <c r="F229" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G229" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
+      </c>
+      <c r="H229" s="10" t="s">
+        <v>422</v>
       </c>
       <c r="I229" s="10">
-        <v>99</v>
+        <v>110</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
@@ -8551,25 +8569,22 @@
         <v>7</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>403</v>
+        <v>432</v>
       </c>
       <c r="D230" s="5">
-        <v>1992</v>
+        <v>1952</v>
       </c>
       <c r="E230" s="9" t="s">
-        <v>404</v>
+        <v>434</v>
       </c>
       <c r="F230" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G230" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H230" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I230" s="10">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
@@ -8580,13 +8595,13 @@
         <v>7</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D231" s="5">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="E231" s="9" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F231" s="9" t="s">
         <v>422</v>
@@ -8598,7 +8613,7 @@
         <v>422</v>
       </c>
       <c r="I231" s="10">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
@@ -8609,25 +8624,25 @@
         <v>7</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="D232" s="5">
-        <v>2012</v>
+        <v>1993</v>
       </c>
       <c r="E232" s="9" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="F232" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G232" s="10" t="s">
         <v>422</v>
       </c>
       <c r="H232" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I232" s="10">
-        <v>143</v>
+        <v>102</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
@@ -8638,10 +8653,10 @@
         <v>7</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D233" s="5">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="E233" s="9" t="s">
         <v>414</v>
@@ -8656,7 +8671,7 @@
         <v>420</v>
       </c>
       <c r="I233" s="10">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
@@ -8667,25 +8682,25 @@
         <v>7</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>107</v>
+        <v>413</v>
       </c>
       <c r="D234" s="5">
-        <v>2002</v>
+        <v>2015</v>
       </c>
       <c r="E234" s="9" t="s">
-        <v>110</v>
+        <v>414</v>
       </c>
       <c r="F234" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G234" s="10" t="s">
         <v>422</v>
       </c>
       <c r="H234" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I234" s="10">
-        <v>116</v>
+        <v>148</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.3">
@@ -8696,10 +8711,10 @@
         <v>7</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D235" s="5">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="E235" s="9" t="s">
         <v>110</v>
@@ -8714,7 +8729,7 @@
         <v>422</v>
       </c>
       <c r="I235" s="10">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.3">
@@ -8725,10 +8740,10 @@
         <v>7</v>
       </c>
       <c r="C236" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D236" s="5">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="E236" s="9" t="s">
         <v>110</v>
@@ -8743,7 +8758,7 @@
         <v>422</v>
       </c>
       <c r="I236" s="10">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
@@ -8754,13 +8769,13 @@
         <v>7</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D237" s="5">
-        <v>2017</v>
+        <v>2007</v>
       </c>
       <c r="E237" s="9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F237" s="9" t="s">
         <v>422</v>
@@ -8769,10 +8784,10 @@
         <v>422</v>
       </c>
       <c r="H237" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I237" s="10">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.3">
@@ -8783,13 +8798,13 @@
         <v>7</v>
       </c>
       <c r="C238" s="3" t="s">
-        <v>362</v>
+        <v>114</v>
       </c>
       <c r="D238" s="5">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E238" s="9" t="s">
-        <v>363</v>
+        <v>115</v>
       </c>
       <c r="F238" s="9" t="s">
         <v>422</v>
@@ -8798,10 +8813,10 @@
         <v>422</v>
       </c>
       <c r="H238" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I238" s="10">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.3">
@@ -8812,13 +8827,13 @@
         <v>7</v>
       </c>
       <c r="C239" s="3" t="s">
-        <v>68</v>
+        <v>362</v>
       </c>
       <c r="D239" s="5">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="E239" s="9" t="s">
-        <v>69</v>
+        <v>363</v>
       </c>
       <c r="F239" s="9" t="s">
         <v>422</v>
@@ -8835,19 +8850,19 @@
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B240" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>460</v>
+        <v>68</v>
       </c>
       <c r="D240" s="5">
-        <v>1999</v>
+        <v>2016</v>
       </c>
       <c r="E240" s="9" t="s">
-        <v>313</v>
+        <v>69</v>
       </c>
       <c r="F240" s="9" t="s">
         <v>422</v>
@@ -8859,7 +8874,7 @@
         <v>422</v>
       </c>
       <c r="I240" s="10">
-        <v>10</v>
+        <v>112</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.3">
@@ -8870,10 +8885,10 @@
         <v>7</v>
       </c>
       <c r="C241" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D241" s="5">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="E241" s="9" t="s">
         <v>313</v>
@@ -8899,10 +8914,10 @@
         <v>7</v>
       </c>
       <c r="C242" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D242" s="5">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="E242" s="9" t="s">
         <v>313</v>
@@ -8928,10 +8943,10 @@
         <v>7</v>
       </c>
       <c r="C243" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D243" s="5">
-        <v>2005</v>
+        <v>2001</v>
       </c>
       <c r="E243" s="9" t="s">
         <v>313</v>
@@ -8957,10 +8972,10 @@
         <v>7</v>
       </c>
       <c r="C244" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D244" s="5">
-        <v>2007</v>
+        <v>2005</v>
       </c>
       <c r="E244" s="9" t="s">
         <v>313</v>
@@ -8986,10 +9001,10 @@
         <v>7</v>
       </c>
       <c r="C245" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D245" s="5">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="E245" s="9" t="s">
         <v>313</v>
@@ -9015,10 +9030,10 @@
         <v>7</v>
       </c>
       <c r="C246" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D246" s="5">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="E246" s="9" t="s">
         <v>313</v>
@@ -9044,10 +9059,10 @@
         <v>7</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D247" s="5">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="E247" s="9" t="s">
         <v>313</v>
@@ -9067,19 +9082,19 @@
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A248" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B248" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>483</v>
+        <v>467</v>
       </c>
       <c r="D248" s="5">
-        <v>2019</v>
+        <v>2011</v>
       </c>
       <c r="E248" s="9" t="s">
-        <v>96</v>
+        <v>313</v>
       </c>
       <c r="F248" s="9" t="s">
         <v>422</v>
@@ -9088,10 +9103,10 @@
         <v>422</v>
       </c>
       <c r="H248" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I248" s="10">
-        <v>141</v>
+        <v>10</v>
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.3">
@@ -9102,10 +9117,10 @@
         <v>49</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>95</v>
+        <v>483</v>
       </c>
       <c r="D249" s="5">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="E249" s="9" t="s">
         <v>96</v>
@@ -9120,7 +9135,7 @@
         <v>420</v>
       </c>
       <c r="I249" s="10">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.3">
@@ -9131,13 +9146,13 @@
         <v>49</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D250" s="5">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E250" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F250" s="9" t="s">
         <v>422</v>
@@ -9149,7 +9164,7 @@
         <v>420</v>
       </c>
       <c r="I250" s="10">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.3">
@@ -9157,16 +9172,16 @@
         <v>416</v>
       </c>
       <c r="B251" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>458</v>
+        <v>97</v>
       </c>
       <c r="D251" s="5">
-        <v>2006</v>
+        <v>2017</v>
       </c>
       <c r="E251" s="9" t="s">
-        <v>459</v>
+        <v>98</v>
       </c>
       <c r="F251" s="9" t="s">
         <v>422</v>
@@ -9175,10 +9190,10 @@
         <v>422</v>
       </c>
       <c r="H251" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I251" s="10">
-        <v>98</v>
+        <v>152</v>
       </c>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.3">
@@ -9189,13 +9204,13 @@
         <v>7</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="D252" s="5">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="E252" s="9" t="s">
-        <v>284</v>
+        <v>459</v>
       </c>
       <c r="F252" s="9" t="s">
         <v>422</v>
@@ -9218,10 +9233,10 @@
         <v>7</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D253" s="5">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="E253" s="9" t="s">
         <v>284</v>
@@ -9236,7 +9251,7 @@
         <v>422</v>
       </c>
       <c r="I253" s="10">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.3">
@@ -9247,13 +9262,13 @@
         <v>7</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>231</v>
+        <v>455</v>
       </c>
       <c r="D254" s="5">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="E254" s="9" t="s">
-        <v>24</v>
+        <v>284</v>
       </c>
       <c r="F254" s="9" t="s">
         <v>422</v>
@@ -9265,7 +9280,7 @@
         <v>422</v>
       </c>
       <c r="I254" s="10">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.3">
@@ -9276,77 +9291,80 @@
         <v>7</v>
       </c>
       <c r="C255" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D255" s="5">
+        <v>2014</v>
+      </c>
+      <c r="E255" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F255" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G255" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H255" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="I255" s="10">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A256" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B256" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C256" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="D255" s="5">
+      <c r="D256" s="5">
         <v>2012</v>
       </c>
-      <c r="E255" s="9" t="s">
+      <c r="E256" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="F255" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="G255" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H255" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="I255" s="10">
+      <c r="F256" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G256" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H256" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="I256" s="10">
         <v>95</v>
       </c>
     </row>
-    <row r="256" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A256" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="B256" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C256" s="3" t="s">
+    <row r="257" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A257" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B257" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C257" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D256" s="5">
+      <c r="D257" s="5">
         <v>2014</v>
       </c>
-      <c r="E256" s="9" t="s">
+      <c r="E257" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="F256" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="G256" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="I256" s="10">
+      <c r="F257" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G257" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="I257" s="10">
         <v>97</v>
-      </c>
-    </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A257" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="B257" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C257" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="D257" s="5">
-        <v>2017</v>
-      </c>
-      <c r="E257" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="F257" s="9" t="s">
-        <v>420</v>
-      </c>
-      <c r="G257" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="I257" s="10">
-        <v>114</v>
       </c>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.3">
@@ -9357,13 +9375,13 @@
         <v>7</v>
       </c>
       <c r="C258" s="3" t="s">
-        <v>497</v>
+        <v>299</v>
       </c>
       <c r="D258" s="5">
         <v>2017</v>
       </c>
       <c r="E258" s="9" t="s">
-        <v>498</v>
+        <v>300</v>
       </c>
       <c r="F258" s="9" t="s">
         <v>420</v>
@@ -9372,7 +9390,7 @@
         <v>420</v>
       </c>
       <c r="I258" s="10">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.3">
@@ -9383,22 +9401,22 @@
         <v>7</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>287</v>
+        <v>497</v>
       </c>
       <c r="D259" s="5">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="E259" s="9" t="s">
-        <v>288</v>
+        <v>498</v>
       </c>
       <c r="F259" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G259" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I259" s="10">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.3">
@@ -9409,22 +9427,22 @@
         <v>7</v>
       </c>
       <c r="C260" s="3" t="s">
-        <v>345</v>
+        <v>287</v>
       </c>
       <c r="D260" s="5">
-        <v>1941</v>
+        <v>2016</v>
       </c>
       <c r="E260" s="9" t="s">
-        <v>347</v>
+        <v>288</v>
       </c>
       <c r="F260" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G260" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I260" s="10">
-        <v>95</v>
+        <v>118</v>
       </c>
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.3">
@@ -9435,22 +9453,22 @@
         <v>7</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>379</v>
+        <v>345</v>
       </c>
       <c r="D261" s="5">
-        <v>2015</v>
+        <v>1941</v>
       </c>
       <c r="E261" s="9" t="s">
-        <v>228</v>
+        <v>347</v>
       </c>
       <c r="F261" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G261" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I261" s="10">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.3">
@@ -9461,13 +9479,13 @@
         <v>7</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>495</v>
+        <v>379</v>
       </c>
       <c r="D262" s="5">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="E262" s="9" t="s">
-        <v>129</v>
+        <v>228</v>
       </c>
       <c r="F262" s="9" t="s">
         <v>422</v>
@@ -9476,7 +9494,7 @@
         <v>420</v>
       </c>
       <c r="I262" s="10">
-        <v>144</v>
+        <v>79</v>
       </c>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.3">
@@ -9487,13 +9505,13 @@
         <v>7</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>73</v>
+        <v>495</v>
       </c>
       <c r="D263" s="5">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="E263" s="9" t="s">
-        <v>74</v>
+        <v>129</v>
       </c>
       <c r="F263" s="9" t="s">
         <v>422</v>
@@ -9502,7 +9520,7 @@
         <v>420</v>
       </c>
       <c r="I263" s="10">
-        <v>91</v>
+        <v>144</v>
       </c>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.3">
@@ -9513,13 +9531,13 @@
         <v>7</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D264" s="5">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="E264" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F264" s="9" t="s">
         <v>422</v>
@@ -9528,7 +9546,7 @@
         <v>420</v>
       </c>
       <c r="I264" s="10">
-        <v>122</v>
+        <v>91</v>
       </c>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.3">
@@ -9539,13 +9557,13 @@
         <v>7</v>
       </c>
       <c r="C265" s="3" t="s">
-        <v>532</v>
+        <v>79</v>
       </c>
       <c r="D265" s="5">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="E265" s="9" t="s">
-        <v>536</v>
+        <v>80</v>
       </c>
       <c r="F265" s="9" t="s">
         <v>422</v>
@@ -9554,7 +9572,7 @@
         <v>420</v>
       </c>
       <c r="I265" s="10">
-        <v>104</v>
+        <v>122</v>
       </c>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.3">
@@ -9565,25 +9583,22 @@
         <v>7</v>
       </c>
       <c r="C266" s="3" t="s">
-        <v>111</v>
+        <v>532</v>
       </c>
       <c r="D266" s="5">
-        <v>2012</v>
+        <v>2019</v>
       </c>
       <c r="E266" s="9" t="s">
-        <v>112</v>
+        <v>536</v>
       </c>
       <c r="F266" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G266" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H266" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I266" s="10">
-        <v>131</v>
+        <v>104</v>
       </c>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.3">
@@ -9594,10 +9609,10 @@
         <v>7</v>
       </c>
       <c r="C267" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D267" s="5">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="E267" s="9" t="s">
         <v>112</v>
@@ -9612,7 +9627,7 @@
         <v>422</v>
       </c>
       <c r="I267" s="10">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.3">
@@ -9620,25 +9635,28 @@
         <v>416</v>
       </c>
       <c r="B268" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C268" s="3" t="s">
-        <v>453</v>
+        <v>113</v>
       </c>
       <c r="D268" s="5">
-        <v>1998</v>
+        <v>2014</v>
       </c>
       <c r="E268" s="9" t="s">
-        <v>393</v>
+        <v>112</v>
       </c>
       <c r="F268" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G268" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
+      </c>
+      <c r="H268" s="10" t="s">
+        <v>422</v>
       </c>
       <c r="I268" s="10">
-        <v>118</v>
+        <v>136</v>
       </c>
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.3">
@@ -9646,16 +9664,16 @@
         <v>416</v>
       </c>
       <c r="B269" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C269" s="3" t="s">
-        <v>585</v>
+        <v>453</v>
       </c>
       <c r="D269" s="5">
-        <v>1985</v>
+        <v>1998</v>
       </c>
       <c r="E269" s="9" t="s">
-        <v>431</v>
+        <v>393</v>
       </c>
       <c r="F269" s="9" t="s">
         <v>422</v>
@@ -9664,7 +9682,7 @@
         <v>420</v>
       </c>
       <c r="I269" s="10">
-        <v>93</v>
+        <v>118</v>
       </c>
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.3">
@@ -9675,22 +9693,22 @@
         <v>7</v>
       </c>
       <c r="C270" s="3" t="s">
-        <v>531</v>
+        <v>585</v>
       </c>
       <c r="D270" s="5">
-        <v>2009</v>
+        <v>1985</v>
       </c>
       <c r="E270" s="9" t="s">
-        <v>188</v>
+        <v>431</v>
       </c>
       <c r="F270" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G270" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I270" s="10">
-        <v>159</v>
+        <v>93</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.3">
@@ -9701,25 +9719,22 @@
         <v>7</v>
       </c>
       <c r="C271" s="3" t="s">
-        <v>480</v>
+        <v>531</v>
       </c>
       <c r="D271" s="5">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="E271" s="9" t="s">
-        <v>72</v>
+        <v>188</v>
       </c>
       <c r="F271" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G271" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H271" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I271" s="10">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.3">
@@ -9730,13 +9745,13 @@
         <v>7</v>
       </c>
       <c r="C272" s="3" t="s">
-        <v>128</v>
+        <v>480</v>
       </c>
       <c r="D272" s="5">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="E272" s="9" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
       <c r="F272" s="9" t="s">
         <v>422</v>
@@ -9745,10 +9760,10 @@
         <v>422</v>
       </c>
       <c r="H272" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I272" s="10">
-        <v>146</v>
+        <v>167</v>
       </c>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.3">
@@ -9759,10 +9774,10 @@
         <v>7</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D273" s="5">
-        <v>2012</v>
+        <v>2008</v>
       </c>
       <c r="E273" s="9" t="s">
         <v>129</v>
@@ -9777,7 +9792,7 @@
         <v>422</v>
       </c>
       <c r="I273" s="10">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.3">
@@ -9785,25 +9800,28 @@
         <v>416</v>
       </c>
       <c r="B274" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C274" s="3" t="s">
-        <v>273</v>
+        <v>130</v>
       </c>
       <c r="D274" s="5">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="E274" s="9" t="s">
-        <v>187</v>
+        <v>129</v>
       </c>
       <c r="F274" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G274" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
+      </c>
+      <c r="H274" s="10" t="s">
+        <v>422</v>
       </c>
       <c r="I274" s="10">
-        <v>113</v>
+        <v>160</v>
       </c>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.3">
@@ -9811,16 +9829,16 @@
         <v>416</v>
       </c>
       <c r="B275" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C275" s="3" t="s">
-        <v>317</v>
+        <v>273</v>
       </c>
       <c r="D275" s="5">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="E275" s="9" t="s">
-        <v>318</v>
+        <v>187</v>
       </c>
       <c r="F275" s="9" t="s">
         <v>422</v>
@@ -9829,7 +9847,7 @@
         <v>420</v>
       </c>
       <c r="I275" s="10">
-        <v>96</v>
+        <v>113</v>
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.3">
@@ -9840,13 +9858,13 @@
         <v>7</v>
       </c>
       <c r="C276" s="3" t="s">
-        <v>385</v>
+        <v>317</v>
       </c>
       <c r="D276" s="5">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="E276" s="9" t="s">
-        <v>386</v>
+        <v>318</v>
       </c>
       <c r="F276" s="9" t="s">
         <v>422</v>
@@ -9855,7 +9873,7 @@
         <v>420</v>
       </c>
       <c r="I276" s="10">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.3">
@@ -9863,25 +9881,25 @@
         <v>416</v>
       </c>
       <c r="B277" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>297</v>
+        <v>385</v>
       </c>
       <c r="D277" s="5">
-        <v>2010</v>
+        <v>2018</v>
       </c>
       <c r="E277" s="9" t="s">
-        <v>298</v>
+        <v>386</v>
       </c>
       <c r="F277" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G277" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I277" s="10">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
@@ -9889,54 +9907,51 @@
         <v>416</v>
       </c>
       <c r="B278" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>380</v>
+        <v>297</v>
       </c>
       <c r="D278" s="5">
-        <v>2018</v>
+        <v>2010</v>
       </c>
       <c r="E278" s="9" t="s">
-        <v>216</v>
+        <v>298</v>
       </c>
       <c r="F278" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G278" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I278" s="10">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A279" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B279" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C279" s="3" t="s">
-        <v>580</v>
+        <v>380</v>
       </c>
       <c r="D279" s="5">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="E279" s="9" t="s">
-        <v>584</v>
+        <v>216</v>
       </c>
       <c r="F279" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G279" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H279" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I279" s="10">
-        <v>22</v>
+        <v>109</v>
       </c>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.3">
@@ -9947,10 +9962,10 @@
         <v>7</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D280" s="5">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E280" s="9" t="s">
         <v>584</v>
@@ -9976,10 +9991,10 @@
         <v>7</v>
       </c>
       <c r="C281" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D281" s="5">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E281" s="9" t="s">
         <v>584</v>
@@ -10005,16 +10020,16 @@
         <v>7</v>
       </c>
       <c r="C282" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D282" s="5">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E282" s="9" t="s">
         <v>584</v>
       </c>
       <c r="F282" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G282" s="10" t="s">
         <v>422</v>
@@ -10028,28 +10043,31 @@
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A283" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B283" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C283" s="3" t="s">
-        <v>222</v>
+        <v>583</v>
       </c>
       <c r="D283" s="5">
-        <v>1985</v>
+        <v>2019</v>
       </c>
       <c r="E283" s="9" t="s">
-        <v>223</v>
+        <v>584</v>
       </c>
       <c r="F283" s="9" t="s">
         <v>420</v>
       </c>
       <c r="G283" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
+      </c>
+      <c r="H283" s="10" t="s">
+        <v>422</v>
       </c>
       <c r="I283" s="10">
-        <v>110</v>
+        <v>22</v>
       </c>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.3">
@@ -10057,25 +10075,25 @@
         <v>416</v>
       </c>
       <c r="B284" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C284" s="3" t="s">
-        <v>302</v>
+        <v>222</v>
       </c>
       <c r="D284" s="5">
-        <v>2014</v>
+        <v>1985</v>
       </c>
       <c r="E284" s="9" t="s">
-        <v>301</v>
+        <v>223</v>
       </c>
       <c r="F284" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G284" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I284" s="10">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.3">
@@ -10086,13 +10104,13 @@
         <v>49</v>
       </c>
       <c r="C285" s="3" t="s">
-        <v>235</v>
+        <v>302</v>
       </c>
       <c r="D285" s="5">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="E285" s="9" t="s">
-        <v>236</v>
+        <v>301</v>
       </c>
       <c r="F285" s="9" t="s">
         <v>422</v>
@@ -10101,7 +10119,7 @@
         <v>420</v>
       </c>
       <c r="I285" s="10">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.3">
@@ -10109,16 +10127,16 @@
         <v>416</v>
       </c>
       <c r="B286" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C286" s="3" t="s">
-        <v>199</v>
+        <v>235</v>
       </c>
       <c r="D286" s="5">
-        <v>2011</v>
+        <v>2017</v>
       </c>
       <c r="E286" s="9" t="s">
-        <v>200</v>
+        <v>236</v>
       </c>
       <c r="F286" s="9" t="s">
         <v>422</v>
@@ -10127,7 +10145,7 @@
         <v>420</v>
       </c>
       <c r="I286" s="10">
-        <v>140</v>
+        <v>105</v>
       </c>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.3">
@@ -10135,25 +10153,25 @@
         <v>416</v>
       </c>
       <c r="B287" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C287" s="3" t="s">
-        <v>503</v>
+        <v>199</v>
       </c>
       <c r="D287" s="5">
-        <v>2020</v>
+        <v>2011</v>
       </c>
       <c r="E287" s="9" t="s">
-        <v>399</v>
+        <v>200</v>
       </c>
       <c r="F287" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G287" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I287" s="10">
-        <v>113</v>
+        <v>140</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.3">
@@ -10161,25 +10179,25 @@
         <v>416</v>
       </c>
       <c r="B288" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C288" s="3" t="s">
-        <v>433</v>
+        <v>503</v>
       </c>
       <c r="D288" s="5">
-        <v>2006</v>
+        <v>2020</v>
       </c>
       <c r="E288" s="9" t="s">
-        <v>218</v>
+        <v>399</v>
       </c>
       <c r="F288" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G288" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I288" s="10">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.3">
@@ -10190,13 +10208,13 @@
         <v>7</v>
       </c>
       <c r="C289" s="3" t="s">
-        <v>351</v>
+        <v>433</v>
       </c>
       <c r="D289" s="5">
-        <v>2002</v>
+        <v>2006</v>
       </c>
       <c r="E289" s="9" t="s">
-        <v>352</v>
+        <v>218</v>
       </c>
       <c r="F289" s="9" t="s">
         <v>422</v>
@@ -10205,7 +10223,7 @@
         <v>420</v>
       </c>
       <c r="I289" s="10">
-        <v>91</v>
+        <v>128</v>
       </c>
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.3">
@@ -10216,13 +10234,13 @@
         <v>7</v>
       </c>
       <c r="C290" s="3" t="s">
-        <v>394</v>
+        <v>351</v>
       </c>
       <c r="D290" s="5">
-        <v>2018</v>
+        <v>2002</v>
       </c>
       <c r="E290" s="9" t="s">
-        <v>395</v>
+        <v>352</v>
       </c>
       <c r="F290" s="9" t="s">
         <v>422</v>
@@ -10231,7 +10249,7 @@
         <v>420</v>
       </c>
       <c r="I290" s="10">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.3">
@@ -10242,25 +10260,22 @@
         <v>7</v>
       </c>
       <c r="C291" s="3" t="s">
-        <v>137</v>
+        <v>394</v>
       </c>
       <c r="D291" s="5">
-        <v>2012</v>
+        <v>2018</v>
       </c>
       <c r="E291" s="9" t="s">
-        <v>47</v>
+        <v>395</v>
       </c>
       <c r="F291" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G291" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H291" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I291" s="10">
-        <v>137</v>
+        <v>101</v>
       </c>
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.3">
@@ -10271,13 +10286,13 @@
         <v>7</v>
       </c>
       <c r="C292" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D292" s="5">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="E292" s="9" t="s">
-        <v>139</v>
+        <v>47</v>
       </c>
       <c r="F292" s="9" t="s">
         <v>422</v>
@@ -10289,7 +10304,7 @@
         <v>422</v>
       </c>
       <c r="I292" s="10">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.3">
@@ -10300,10 +10315,10 @@
         <v>7</v>
       </c>
       <c r="C293" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D293" s="5">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="E293" s="9" t="s">
         <v>139</v>
@@ -10318,7 +10333,7 @@
         <v>422</v>
       </c>
       <c r="I293" s="10">
-        <v>118</v>
+        <v>141</v>
       </c>
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.3">
@@ -10329,10 +10344,10 @@
         <v>7</v>
       </c>
       <c r="C294" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D294" s="5">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="E294" s="9" t="s">
         <v>139</v>
@@ -10347,7 +10362,7 @@
         <v>422</v>
       </c>
       <c r="I294" s="10">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.3">
@@ -10358,13 +10373,13 @@
         <v>7</v>
       </c>
       <c r="C295" s="3" t="s">
-        <v>239</v>
+        <v>142</v>
       </c>
       <c r="D295" s="5">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="E295" s="9" t="s">
-        <v>240</v>
+        <v>139</v>
       </c>
       <c r="F295" s="9" t="s">
         <v>422</v>
@@ -10373,10 +10388,10 @@
         <v>422</v>
       </c>
       <c r="H295" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I295" s="10">
-        <v>109</v>
+        <v>132</v>
       </c>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.3">
@@ -10387,22 +10402,25 @@
         <v>7</v>
       </c>
       <c r="C296" s="3" t="s">
-        <v>443</v>
+        <v>239</v>
       </c>
       <c r="D296" s="5">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="E296" s="9" t="s">
-        <v>445</v>
+        <v>240</v>
       </c>
       <c r="F296" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G296" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H296" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I296" s="10">
-        <v>90</v>
+        <v>109</v>
       </c>
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.3">
@@ -10413,13 +10431,13 @@
         <v>7</v>
       </c>
       <c r="C297" s="3" t="s">
-        <v>196</v>
+        <v>443</v>
       </c>
       <c r="D297" s="5">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="E297" s="9" t="s">
-        <v>172</v>
+        <v>445</v>
       </c>
       <c r="F297" s="9" t="s">
         <v>422</v>
@@ -10428,7 +10446,7 @@
         <v>420</v>
       </c>
       <c r="I297" s="10">
-        <v>110</v>
+        <v>90</v>
       </c>
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.3">
@@ -10439,13 +10457,13 @@
         <v>7</v>
       </c>
       <c r="C298" s="3" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="D298" s="5">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="E298" s="9" t="s">
-        <v>218</v>
+        <v>172</v>
       </c>
       <c r="F298" s="9" t="s">
         <v>422</v>
@@ -10454,7 +10472,7 @@
         <v>420</v>
       </c>
       <c r="I298" s="10">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="299" spans="1:11" x14ac:dyDescent="0.3">
@@ -10465,19 +10483,22 @@
         <v>7</v>
       </c>
       <c r="C299" s="3" t="s">
-        <v>597</v>
+        <v>217</v>
       </c>
       <c r="D299" s="5">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E299" s="9" t="s">
-        <v>440</v>
+        <v>218</v>
       </c>
       <c r="F299" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G299" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I299" s="10">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="300" spans="1:11" x14ac:dyDescent="0.3">
@@ -10485,25 +10506,22 @@
         <v>416</v>
       </c>
       <c r="B300" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C300" s="3" t="s">
-        <v>305</v>
+        <v>597</v>
       </c>
       <c r="D300" s="5">
-        <v>2010</v>
+        <v>2017</v>
       </c>
       <c r="E300" s="9" t="s">
-        <v>306</v>
+        <v>440</v>
       </c>
       <c r="F300" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="G300" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I300" s="10">
-        <v>140</v>
+        <v>105</v>
       </c>
     </row>
     <row r="301" spans="1:11" x14ac:dyDescent="0.3">
@@ -10514,13 +10532,13 @@
         <v>49</v>
       </c>
       <c r="C301" s="3" t="s">
-        <v>602</v>
+        <v>305</v>
       </c>
       <c r="D301" s="5">
-        <v>2021</v>
+        <v>2010</v>
       </c>
       <c r="E301" s="9" t="s">
-        <v>170</v>
+        <v>306</v>
       </c>
       <c r="F301" s="9" t="s">
         <v>422</v>
@@ -10529,10 +10547,7 @@
         <v>420</v>
       </c>
       <c r="I301" s="10">
-        <v>152</v>
-      </c>
-      <c r="K301" t="s">
-        <v>603</v>
+        <v>140</v>
       </c>
     </row>
     <row r="302" spans="1:11" x14ac:dyDescent="0.3">
@@ -10540,25 +10555,28 @@
         <v>416</v>
       </c>
       <c r="B302" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C302" s="3" t="s">
-        <v>447</v>
+        <v>602</v>
       </c>
       <c r="D302" s="5">
-        <v>2007</v>
+        <v>2021</v>
       </c>
       <c r="E302" s="9" t="s">
-        <v>446</v>
+        <v>170</v>
       </c>
       <c r="F302" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G302" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I302" s="10">
-        <v>118</v>
+        <v>152</v>
+      </c>
+      <c r="K302" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="303" spans="1:11" x14ac:dyDescent="0.3">
@@ -10566,25 +10584,25 @@
         <v>416</v>
       </c>
       <c r="B303" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C303" s="3" t="s">
-        <v>538</v>
+        <v>447</v>
       </c>
       <c r="D303" s="5">
-        <v>2016</v>
+        <v>2007</v>
       </c>
       <c r="E303" s="9" t="s">
-        <v>153</v>
+        <v>446</v>
       </c>
       <c r="F303" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G303" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I303" s="10">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="304" spans="1:11" x14ac:dyDescent="0.3">
@@ -10595,22 +10613,22 @@
         <v>49</v>
       </c>
       <c r="C304" s="3" t="s">
-        <v>499</v>
+        <v>538</v>
       </c>
       <c r="D304" s="5">
         <v>2016</v>
       </c>
       <c r="E304" s="9" t="s">
-        <v>500</v>
+        <v>153</v>
       </c>
       <c r="F304" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G304" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I304" s="10">
-        <v>133</v>
+        <v>110</v>
       </c>
     </row>
     <row r="305" spans="1:9" x14ac:dyDescent="0.3">
@@ -10618,28 +10636,25 @@
         <v>416</v>
       </c>
       <c r="B305" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C305" s="3" t="s">
-        <v>100</v>
+        <v>499</v>
       </c>
       <c r="D305" s="5">
-        <v>1997</v>
+        <v>2016</v>
       </c>
       <c r="E305" s="9" t="s">
-        <v>91</v>
+        <v>500</v>
       </c>
       <c r="F305" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G305" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H305" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I305" s="10">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.3">
@@ -10647,25 +10662,28 @@
         <v>416</v>
       </c>
       <c r="B306" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C306" s="3" t="s">
-        <v>169</v>
+        <v>100</v>
       </c>
       <c r="D306" s="5">
-        <v>2015</v>
+        <v>1997</v>
       </c>
       <c r="E306" s="9" t="s">
-        <v>170</v>
+        <v>91</v>
       </c>
       <c r="F306" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G306" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
+      </c>
+      <c r="H306" s="10" t="s">
+        <v>422</v>
       </c>
       <c r="I306" s="10">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.3">
@@ -10673,16 +10691,16 @@
         <v>416</v>
       </c>
       <c r="B307" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C307" s="3" t="s">
-        <v>565</v>
+        <v>169</v>
       </c>
       <c r="D307" s="5">
-        <v>2021</v>
+        <v>2015</v>
       </c>
       <c r="E307" s="9" t="s">
-        <v>446</v>
+        <v>170</v>
       </c>
       <c r="F307" s="9" t="s">
         <v>422</v>
@@ -10691,7 +10709,7 @@
         <v>420</v>
       </c>
       <c r="I307" s="10">
-        <v>124</v>
+        <v>142</v>
       </c>
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.3">
@@ -10702,25 +10720,22 @@
         <v>7</v>
       </c>
       <c r="C308" s="3" t="s">
-        <v>165</v>
+        <v>565</v>
       </c>
       <c r="D308" s="5">
-        <v>2014</v>
+        <v>2021</v>
       </c>
       <c r="E308" s="9" t="s">
-        <v>166</v>
+        <v>446</v>
       </c>
       <c r="F308" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G308" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H308" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I308" s="10">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.3">
@@ -10731,22 +10746,25 @@
         <v>7</v>
       </c>
       <c r="C309" s="3" t="s">
-        <v>56</v>
+        <v>165</v>
       </c>
       <c r="D309" s="5">
-        <v>1980</v>
+        <v>2014</v>
       </c>
       <c r="E309" s="9" t="s">
-        <v>55</v>
+        <v>166</v>
       </c>
       <c r="F309" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G309" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H309" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I309" s="10">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.3">
@@ -10757,65 +10775,65 @@
         <v>7</v>
       </c>
       <c r="C310" s="3" t="s">
-        <v>226</v>
+        <v>56</v>
       </c>
       <c r="D310" s="5">
-        <v>1999</v>
+        <v>1980</v>
       </c>
       <c r="E310" s="9" t="s">
-        <v>227</v>
+        <v>55</v>
       </c>
       <c r="F310" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G310" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I310" s="10">
-        <v>120</v>
+        <v>101</v>
       </c>
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A311" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B311" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C311" s="3" t="s">
-        <v>553</v>
+        <v>226</v>
       </c>
       <c r="D311" s="5">
-        <v>2016</v>
+        <v>1999</v>
       </c>
       <c r="E311" s="9" t="s">
-        <v>557</v>
+        <v>227</v>
       </c>
       <c r="F311" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G311" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I311" s="10">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A312" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B312" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C312" s="3" t="s">
-        <v>323</v>
+        <v>553</v>
       </c>
       <c r="D312" s="5">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="E312" s="9" t="s">
-        <v>324</v>
+        <v>557</v>
       </c>
       <c r="F312" s="9" t="s">
         <v>422</v>
@@ -10824,7 +10842,7 @@
         <v>420</v>
       </c>
       <c r="I312" s="10">
-        <v>99</v>
+        <v>60</v>
       </c>
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.3">
@@ -10832,28 +10850,25 @@
         <v>416</v>
       </c>
       <c r="B313" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C313" s="3" t="s">
-        <v>425</v>
+        <v>323</v>
       </c>
       <c r="D313" s="5">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="E313" s="9" t="s">
-        <v>214</v>
+        <v>324</v>
       </c>
       <c r="F313" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G313" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H313" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I313" s="10">
-        <v>119</v>
+        <v>99</v>
       </c>
     </row>
     <row r="314" spans="1:9" x14ac:dyDescent="0.3">
@@ -10864,22 +10879,25 @@
         <v>7</v>
       </c>
       <c r="C314" s="3" t="s">
-        <v>315</v>
+        <v>425</v>
       </c>
       <c r="D314" s="5">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="E314" s="9" t="s">
-        <v>316</v>
+        <v>214</v>
       </c>
       <c r="F314" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G314" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H314" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I314" s="10">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.3">
@@ -10890,13 +10908,13 @@
         <v>7</v>
       </c>
       <c r="C315" s="3" t="s">
-        <v>262</v>
+        <v>315</v>
       </c>
       <c r="D315" s="5">
-        <v>2007</v>
+        <v>2017</v>
       </c>
       <c r="E315" s="9" t="s">
-        <v>266</v>
+        <v>316</v>
       </c>
       <c r="F315" s="9" t="s">
         <v>422</v>
@@ -10905,7 +10923,7 @@
         <v>420</v>
       </c>
       <c r="I315" s="10">
-        <v>83</v>
+        <v>118</v>
       </c>
     </row>
     <row r="316" spans="1:9" x14ac:dyDescent="0.3">
@@ -10916,74 +10934,74 @@
         <v>7</v>
       </c>
       <c r="C316" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D316" s="5">
+        <v>2007</v>
+      </c>
+      <c r="E316" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="F316" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G316" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="I316" s="10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A317" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B317" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C317" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="D316" s="5">
+      <c r="D317" s="5">
         <v>1965</v>
       </c>
-      <c r="E316" s="9" t="s">
+      <c r="E317" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="F316" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="G316" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="I316" s="10">
+      <c r="F317" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G317" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="I317" s="10">
         <v>168</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A317" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="B317" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C317" s="3" t="s">
+    <row r="318" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A318" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B318" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C318" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="D317" s="5">
+      <c r="D318" s="5">
         <v>2004</v>
       </c>
-      <c r="E317" s="9" t="s">
+      <c r="E318" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="F317" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="G317" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="I317" s="10">
+      <c r="F318" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G318" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="I318" s="10">
         <v>83</v>
-      </c>
-    </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A318" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="B318" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C318" s="3" t="s">
-        <v>554</v>
-      </c>
-      <c r="D318" s="5">
-        <v>2021</v>
-      </c>
-      <c r="E318" s="9" t="s">
-        <v>555</v>
-      </c>
-      <c r="F318" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="G318" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="I318" s="10">
-        <v>132</v>
       </c>
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.3">
@@ -10991,16 +11009,16 @@
         <v>416</v>
       </c>
       <c r="B319" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C319" s="3" t="s">
-        <v>195</v>
+        <v>554</v>
       </c>
       <c r="D319" s="5">
-        <v>2014</v>
+        <v>2021</v>
       </c>
       <c r="E319" s="9" t="s">
-        <v>194</v>
+        <v>555</v>
       </c>
       <c r="F319" s="9" t="s">
         <v>422</v>
@@ -11009,7 +11027,7 @@
         <v>420</v>
       </c>
       <c r="I319" s="10">
-        <v>118</v>
+        <v>132</v>
       </c>
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.3">
@@ -11020,13 +11038,13 @@
         <v>7</v>
       </c>
       <c r="C320" s="3" t="s">
-        <v>426</v>
+        <v>195</v>
       </c>
       <c r="D320" s="5">
-        <v>1998</v>
+        <v>2014</v>
       </c>
       <c r="E320" s="9" t="s">
-        <v>429</v>
+        <v>194</v>
       </c>
       <c r="F320" s="9" t="s">
         <v>422</v>
@@ -11035,24 +11053,24 @@
         <v>420</v>
       </c>
       <c r="I320" s="10">
-        <v>99</v>
+        <v>118</v>
       </c>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A321" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B321" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C321" s="3" t="s">
-        <v>607</v>
+        <v>426</v>
       </c>
       <c r="D321" s="5">
-        <v>2017</v>
+        <v>1998</v>
       </c>
       <c r="E321" s="9" t="s">
-        <v>608</v>
+        <v>429</v>
       </c>
       <c r="F321" s="9" t="s">
         <v>422</v>
@@ -11061,24 +11079,24 @@
         <v>420</v>
       </c>
       <c r="I321" s="10">
-        <v>60</v>
+        <v>99</v>
       </c>
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A322" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B322" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C322" s="3" t="s">
-        <v>189</v>
+        <v>607</v>
       </c>
       <c r="D322" s="5">
         <v>2017</v>
       </c>
       <c r="E322" s="9" t="s">
-        <v>190</v>
+        <v>608</v>
       </c>
       <c r="F322" s="9" t="s">
         <v>422</v>
@@ -11087,7 +11105,7 @@
         <v>420</v>
       </c>
       <c r="I322" s="10">
-        <v>122</v>
+        <v>60</v>
       </c>
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.3">
@@ -11098,22 +11116,22 @@
         <v>7</v>
       </c>
       <c r="C323" s="3" t="s">
-        <v>563</v>
+        <v>189</v>
       </c>
       <c r="D323" s="5">
-        <v>2001</v>
+        <v>2017</v>
       </c>
       <c r="E323" s="9" t="s">
-        <v>564</v>
+        <v>190</v>
       </c>
       <c r="F323" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G323" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I323" s="10">
-        <v>90</v>
+        <v>122</v>
       </c>
     </row>
     <row r="324" spans="1:9" x14ac:dyDescent="0.3">
@@ -11121,28 +11139,25 @@
         <v>416</v>
       </c>
       <c r="B324" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C324" s="3" t="s">
-        <v>118</v>
+        <v>563</v>
       </c>
       <c r="D324" s="5">
-        <v>2017</v>
+        <v>2001</v>
       </c>
       <c r="E324" s="9" t="s">
-        <v>119</v>
+        <v>564</v>
       </c>
       <c r="F324" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G324" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H324" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I324" s="10">
-        <v>130</v>
+        <v>90</v>
       </c>
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.3">
@@ -11153,22 +11168,25 @@
         <v>49</v>
       </c>
       <c r="C325" s="3" t="s">
-        <v>167</v>
+        <v>118</v>
       </c>
       <c r="D325" s="5">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="E325" s="9" t="s">
-        <v>168</v>
+        <v>119</v>
       </c>
       <c r="F325" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G325" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H325" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I325" s="10">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.3">
@@ -11179,25 +11197,22 @@
         <v>7</v>
       </c>
       <c r="C326" s="3" t="s">
-        <v>77</v>
+        <v>614</v>
       </c>
       <c r="D326" s="5">
-        <v>1986</v>
+        <v>2022</v>
       </c>
       <c r="E326" s="9" t="s">
-        <v>78</v>
+        <v>615</v>
       </c>
       <c r="F326" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G326" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H326" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I326" s="10">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.3">
@@ -11205,28 +11220,25 @@
         <v>416</v>
       </c>
       <c r="B327" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C327" s="3" t="s">
-        <v>575</v>
+        <v>167</v>
       </c>
       <c r="D327" s="5">
-        <v>1995</v>
+        <v>2018</v>
       </c>
       <c r="E327" s="9" t="s">
-        <v>576</v>
+        <v>168</v>
       </c>
       <c r="F327" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G327" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H327" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I327" s="10">
-        <v>78</v>
+        <v>118</v>
       </c>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.3">
@@ -11237,16 +11249,16 @@
         <v>7</v>
       </c>
       <c r="C328" s="3" t="s">
-        <v>574</v>
+        <v>77</v>
       </c>
       <c r="D328" s="5">
-        <v>1999</v>
+        <v>1986</v>
       </c>
       <c r="E328" s="9" t="s">
-        <v>576</v>
+        <v>78</v>
       </c>
       <c r="F328" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G328" s="10" t="s">
         <v>422</v>
@@ -11255,7 +11267,7 @@
         <v>420</v>
       </c>
       <c r="I328" s="10">
-        <v>89</v>
+        <v>105</v>
       </c>
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.3">
@@ -11266,13 +11278,13 @@
         <v>7</v>
       </c>
       <c r="C329" s="3" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="D329" s="5">
-        <v>2010</v>
+        <v>1995</v>
       </c>
       <c r="E329" s="9" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F329" s="9" t="s">
         <v>422</v>
@@ -11284,7 +11296,7 @@
         <v>420</v>
       </c>
       <c r="I329" s="10">
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.3">
@@ -11295,13 +11307,13 @@
         <v>7</v>
       </c>
       <c r="C330" s="3" t="s">
-        <v>261</v>
+        <v>574</v>
       </c>
       <c r="D330" s="5">
-        <v>2016</v>
+        <v>1999</v>
       </c>
       <c r="E330" s="9" t="s">
-        <v>263</v>
+        <v>576</v>
       </c>
       <c r="F330" s="9" t="s">
         <v>422</v>
@@ -11313,7 +11325,7 @@
         <v>420</v>
       </c>
       <c r="I330" s="10">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.3">
@@ -11324,22 +11336,25 @@
         <v>7</v>
       </c>
       <c r="C331" s="3" t="s">
-        <v>392</v>
+        <v>573</v>
       </c>
       <c r="D331" s="5">
         <v>2010</v>
       </c>
       <c r="E331" s="9" t="s">
-        <v>393</v>
+        <v>577</v>
       </c>
       <c r="F331" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G331" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H331" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I331" s="10">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.3">
@@ -11350,13 +11365,13 @@
         <v>7</v>
       </c>
       <c r="C332" s="3" t="s">
-        <v>70</v>
+        <v>261</v>
       </c>
       <c r="D332" s="5">
-        <v>2000</v>
+        <v>2016</v>
       </c>
       <c r="E332" s="9" t="s">
-        <v>69</v>
+        <v>263</v>
       </c>
       <c r="F332" s="9" t="s">
         <v>422</v>
@@ -11365,10 +11380,10 @@
         <v>422</v>
       </c>
       <c r="H332" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I332" s="10">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.3">
@@ -11379,22 +11394,25 @@
         <v>7</v>
       </c>
       <c r="C333" s="3" t="s">
-        <v>215</v>
+        <v>612</v>
       </c>
       <c r="D333" s="5">
-        <v>2009</v>
+        <v>2020</v>
       </c>
       <c r="E333" s="9" t="s">
-        <v>216</v>
+        <v>613</v>
       </c>
       <c r="F333" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G333" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H333" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I333" s="10">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.3">
@@ -11405,13 +11423,13 @@
         <v>7</v>
       </c>
       <c r="C334" s="3" t="s">
-        <v>355</v>
+        <v>392</v>
       </c>
       <c r="D334" s="5">
-        <v>2019</v>
+        <v>2010</v>
       </c>
       <c r="E334" s="9" t="s">
-        <v>67</v>
+        <v>393</v>
       </c>
       <c r="F334" s="9" t="s">
         <v>422</v>
@@ -11420,7 +11438,7 @@
         <v>420</v>
       </c>
       <c r="I334" s="10">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.3">
@@ -11431,13 +11449,13 @@
         <v>7</v>
       </c>
       <c r="C335" s="3" t="s">
-        <v>361</v>
+        <v>70</v>
       </c>
       <c r="D335" s="5">
-        <v>2018</v>
+        <v>2000</v>
       </c>
       <c r="E335" s="9" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="F335" s="9" t="s">
         <v>422</v>
@@ -11446,10 +11464,10 @@
         <v>422</v>
       </c>
       <c r="H335" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I335" s="10">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.3">
@@ -11460,13 +11478,13 @@
         <v>7</v>
       </c>
       <c r="C336" s="3" t="s">
-        <v>381</v>
+        <v>215</v>
       </c>
       <c r="D336" s="5">
-        <v>2018</v>
+        <v>2009</v>
       </c>
       <c r="E336" s="9" t="s">
-        <v>382</v>
+        <v>216</v>
       </c>
       <c r="F336" s="9" t="s">
         <v>422</v>
@@ -11475,7 +11493,7 @@
         <v>420</v>
       </c>
       <c r="I336" s="10">
-        <v>129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.3">
@@ -11486,13 +11504,13 @@
         <v>7</v>
       </c>
       <c r="C337" s="3" t="s">
-        <v>43</v>
+        <v>355</v>
       </c>
       <c r="D337" s="5">
-        <v>1998</v>
+        <v>2019</v>
       </c>
       <c r="E337" s="9" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="F337" s="9" t="s">
         <v>422</v>
@@ -11501,7 +11519,7 @@
         <v>420</v>
       </c>
       <c r="I337" s="10">
-        <v>87</v>
+        <v>111</v>
       </c>
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.3">
@@ -11509,16 +11527,16 @@
         <v>416</v>
       </c>
       <c r="B338" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C338" s="3" t="s">
-        <v>517</v>
+        <v>361</v>
       </c>
       <c r="D338" s="5">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="E338" s="9" t="s">
-        <v>518</v>
+        <v>59</v>
       </c>
       <c r="F338" s="9" t="s">
         <v>422</v>
@@ -11530,24 +11548,24 @@
         <v>420</v>
       </c>
       <c r="I338" s="10">
-        <v>140</v>
+        <v>108</v>
       </c>
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A339" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B339" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C339" s="3" t="s">
-        <v>528</v>
+        <v>381</v>
       </c>
       <c r="D339" s="5">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="E339" s="9" t="s">
-        <v>533</v>
+        <v>382</v>
       </c>
       <c r="F339" s="9" t="s">
         <v>422</v>
@@ -11556,7 +11574,7 @@
         <v>420</v>
       </c>
       <c r="I339" s="10">
-        <v>56</v>
+        <v>129</v>
       </c>
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.3">
@@ -11567,13 +11585,13 @@
         <v>7</v>
       </c>
       <c r="C340" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D340" s="5">
-        <v>2013</v>
+        <v>1998</v>
       </c>
       <c r="E340" s="9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F340" s="9" t="s">
         <v>422</v>
@@ -11582,7 +11600,7 @@
         <v>420</v>
       </c>
       <c r="I340" s="10">
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.3">
@@ -11590,42 +11608,45 @@
         <v>416</v>
       </c>
       <c r="B341" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C341" s="3" t="s">
-        <v>508</v>
+        <v>517</v>
       </c>
       <c r="D341" s="5">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E341" s="9" t="s">
-        <v>507</v>
+        <v>518</v>
       </c>
       <c r="F341" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G341" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H341" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I341" s="10">
-        <v>105</v>
+        <v>140</v>
       </c>
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A342" s="3" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B342" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C342" s="3" t="s">
-        <v>233</v>
+        <v>528</v>
       </c>
       <c r="D342" s="5">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="E342" s="9" t="s">
-        <v>234</v>
+        <v>533</v>
       </c>
       <c r="F342" s="9" t="s">
         <v>422</v>
@@ -11634,7 +11655,7 @@
         <v>420</v>
       </c>
       <c r="I342" s="10">
-        <v>107</v>
+        <v>56</v>
       </c>
     </row>
     <row r="343" spans="1:9" x14ac:dyDescent="0.3">
@@ -11645,13 +11666,13 @@
         <v>7</v>
       </c>
       <c r="C343" s="3" t="s">
-        <v>418</v>
+        <v>39</v>
       </c>
       <c r="D343" s="5">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="E343" s="9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F343" s="9" t="s">
         <v>422</v>
@@ -11660,7 +11681,7 @@
         <v>420</v>
       </c>
       <c r="I343" s="10">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.3">
@@ -11671,13 +11692,13 @@
         <v>7</v>
       </c>
       <c r="C344" s="3" t="s">
-        <v>75</v>
+        <v>508</v>
       </c>
       <c r="D344" s="5">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="E344" s="9" t="s">
-        <v>76</v>
+        <v>507</v>
       </c>
       <c r="F344" s="9" t="s">
         <v>422</v>
@@ -11686,7 +11707,7 @@
         <v>420</v>
       </c>
       <c r="I344" s="10">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.3">
@@ -11694,16 +11715,16 @@
         <v>416</v>
       </c>
       <c r="B345" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C345" s="3" t="s">
-        <v>373</v>
+        <v>233</v>
       </c>
       <c r="D345" s="5">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="E345" s="9" t="s">
-        <v>374</v>
+        <v>234</v>
       </c>
       <c r="F345" s="9" t="s">
         <v>422</v>
@@ -11712,7 +11733,7 @@
         <v>420</v>
       </c>
       <c r="I345" s="10">
-        <v>124</v>
+        <v>107</v>
       </c>
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.3">
@@ -11720,25 +11741,25 @@
         <v>416</v>
       </c>
       <c r="B346" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C346" s="3" t="s">
-        <v>358</v>
+        <v>418</v>
       </c>
       <c r="D346" s="5">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="E346" s="9" t="s">
-        <v>359</v>
+        <v>32</v>
       </c>
       <c r="F346" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G346" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I346" s="10">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.3">
@@ -11749,22 +11770,22 @@
         <v>7</v>
       </c>
       <c r="C347" s="3" t="s">
-        <v>566</v>
+        <v>75</v>
       </c>
       <c r="D347" s="5">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="E347" s="9" t="s">
-        <v>567</v>
+        <v>76</v>
       </c>
       <c r="F347" s="9" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G347" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I347" s="10">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.3">
@@ -11775,25 +11796,22 @@
         <v>7</v>
       </c>
       <c r="C348" s="3" t="s">
-        <v>291</v>
+        <v>373</v>
       </c>
       <c r="D348" s="5">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="E348" s="9" t="s">
-        <v>292</v>
+        <v>374</v>
       </c>
       <c r="F348" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G348" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H348" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I348" s="10">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.3">
@@ -11804,25 +11822,22 @@
         <v>49</v>
       </c>
       <c r="C349" s="3" t="s">
-        <v>511</v>
+        <v>358</v>
       </c>
       <c r="D349" s="5">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="E349" s="9" t="s">
-        <v>292</v>
+        <v>359</v>
       </c>
       <c r="F349" s="9" t="s">
         <v>420</v>
       </c>
       <c r="G349" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H349" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I349" s="10">
-        <v>153</v>
+        <v>109</v>
       </c>
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.3">
@@ -11833,22 +11848,22 @@
         <v>7</v>
       </c>
       <c r="C350" s="3" t="s">
-        <v>62</v>
+        <v>566</v>
       </c>
       <c r="D350" s="5">
-        <v>2013</v>
+        <v>2017</v>
       </c>
       <c r="E350" s="9" t="s">
-        <v>63</v>
+        <v>567</v>
       </c>
       <c r="F350" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G350" s="10" t="s">
         <v>420</v>
       </c>
       <c r="I350" s="10">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.3">
@@ -11859,13 +11874,13 @@
         <v>7</v>
       </c>
       <c r="C351" s="3" t="s">
-        <v>126</v>
+        <v>291</v>
       </c>
       <c r="D351" s="5">
-        <v>2000</v>
+        <v>2017</v>
       </c>
       <c r="E351" s="9" t="s">
-        <v>121</v>
+        <v>292</v>
       </c>
       <c r="F351" s="9" t="s">
         <v>422</v>
@@ -11877,7 +11892,7 @@
         <v>422</v>
       </c>
       <c r="I351" s="10">
-        <v>100</v>
+        <v>135</v>
       </c>
     </row>
     <row r="352" spans="1:9" x14ac:dyDescent="0.3">
@@ -11885,19 +11900,19 @@
         <v>416</v>
       </c>
       <c r="B352" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C352" s="3" t="s">
-        <v>127</v>
+        <v>511</v>
       </c>
       <c r="D352" s="5">
-        <v>2003</v>
+        <v>2020</v>
       </c>
       <c r="E352" s="9" t="s">
-        <v>121</v>
+        <v>292</v>
       </c>
       <c r="F352" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G352" s="10" t="s">
         <v>422</v>
@@ -11906,7 +11921,7 @@
         <v>422</v>
       </c>
       <c r="I352" s="10">
-        <v>128</v>
+        <v>153</v>
       </c>
     </row>
     <row r="353" spans="1:9" x14ac:dyDescent="0.3">
@@ -11917,25 +11932,22 @@
         <v>7</v>
       </c>
       <c r="C353" s="3" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="D353" s="5">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="E353" s="9" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="F353" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G353" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H353" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I353" s="10">
-        <v>138</v>
+        <v>112</v>
       </c>
     </row>
     <row r="354" spans="1:9" x14ac:dyDescent="0.3">
@@ -11946,13 +11958,13 @@
         <v>7</v>
       </c>
       <c r="C354" s="3" t="s">
-        <v>479</v>
+        <v>126</v>
       </c>
       <c r="D354" s="5">
-        <v>2019</v>
+        <v>2000</v>
       </c>
       <c r="E354" s="9" t="s">
-        <v>481</v>
+        <v>121</v>
       </c>
       <c r="F354" s="9" t="s">
         <v>422</v>
@@ -11964,7 +11976,7 @@
         <v>422</v>
       </c>
       <c r="I354" s="10">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="355" spans="1:9" x14ac:dyDescent="0.3">
@@ -11975,10 +11987,10 @@
         <v>7</v>
       </c>
       <c r="C355" s="3" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D355" s="5">
-        <v>2014</v>
+        <v>2003</v>
       </c>
       <c r="E355" s="9" t="s">
         <v>121</v>
@@ -11993,7 +12005,7 @@
         <v>422</v>
       </c>
       <c r="I355" s="10">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="356" spans="1:9" x14ac:dyDescent="0.3">
@@ -12004,13 +12016,13 @@
         <v>7</v>
       </c>
       <c r="C356" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D356" s="5">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="E356" s="9" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="F356" s="9" t="s">
         <v>422</v>
@@ -12022,7 +12034,7 @@
         <v>422</v>
       </c>
       <c r="I356" s="10">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="357" spans="1:9" x14ac:dyDescent="0.3">
@@ -12033,13 +12045,13 @@
         <v>7</v>
       </c>
       <c r="C357" s="3" t="s">
-        <v>124</v>
+        <v>479</v>
       </c>
       <c r="D357" s="5">
-        <v>2006</v>
+        <v>2019</v>
       </c>
       <c r="E357" s="9" t="s">
-        <v>125</v>
+        <v>481</v>
       </c>
       <c r="F357" s="9" t="s">
         <v>422</v>
@@ -12051,7 +12063,7 @@
         <v>422</v>
       </c>
       <c r="I357" s="10">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="358" spans="1:9" x14ac:dyDescent="0.3">
@@ -12059,25 +12071,28 @@
         <v>416</v>
       </c>
       <c r="B358" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C358" s="3" t="s">
-        <v>516</v>
+        <v>122</v>
       </c>
       <c r="D358" s="5">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="E358" s="9" t="s">
-        <v>519</v>
+        <v>121</v>
       </c>
       <c r="F358" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G358" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
+      </c>
+      <c r="H358" s="10" t="s">
+        <v>422</v>
       </c>
       <c r="I358" s="10">
-        <v>98</v>
+        <v>126</v>
       </c>
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.3">
@@ -12085,25 +12100,28 @@
         <v>416</v>
       </c>
       <c r="B359" s="7" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="C359" s="3" t="s">
-        <v>524</v>
+        <v>123</v>
       </c>
       <c r="D359" s="5">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="E359" s="9" t="s">
-        <v>525</v>
+        <v>84</v>
       </c>
       <c r="F359" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G359" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
+      </c>
+      <c r="H359" s="10" t="s">
+        <v>422</v>
       </c>
       <c r="I359" s="10">
-        <v>157</v>
+        <v>126</v>
       </c>
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.3">
@@ -12114,13 +12132,13 @@
         <v>7</v>
       </c>
       <c r="C360" s="3" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="D360" s="5">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="E360" s="9" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
       <c r="F360" s="9" t="s">
         <v>422</v>
@@ -12132,7 +12150,7 @@
         <v>422</v>
       </c>
       <c r="I360" s="10">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="361" spans="1:9" x14ac:dyDescent="0.3">
@@ -12143,25 +12161,22 @@
         <v>49</v>
       </c>
       <c r="C361" s="3" t="s">
-        <v>360</v>
+        <v>516</v>
       </c>
       <c r="D361" s="5">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="E361" s="9" t="s">
-        <v>59</v>
+        <v>519</v>
       </c>
       <c r="F361" s="9" t="s">
         <v>422</v>
       </c>
       <c r="G361" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="H361" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I361" s="10">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.3">
@@ -12169,30 +12184,114 @@
         <v>416</v>
       </c>
       <c r="B362" s="7" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C362" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="D362" s="5">
+        <v>2012</v>
+      </c>
+      <c r="E362" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="F362" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G362" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="I362" s="10">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="363" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A363" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B363" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C363" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D363" s="5">
+        <v>2009</v>
+      </c>
+      <c r="E363" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F363" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G363" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H363" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="I363" s="10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="364" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A364" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B364" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C364" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="D364" s="5">
+        <v>2019</v>
+      </c>
+      <c r="E364" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F364" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G364" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H364" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="I364" s="10">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="365" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A365" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B365" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C365" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D362" s="5">
+      <c r="D365" s="5">
         <v>2016</v>
       </c>
-      <c r="E362" s="9" t="s">
+      <c r="E365" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="F362" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="G362" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="I362" s="10">
+      <c r="F365" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="G365" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="I365" s="10">
         <v>104</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:L1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L362">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L365">
       <sortCondition ref="C1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
update the end we start from, sharp objects, succcession
</commit_message>
<xml_diff>
--- a/src/data/database.xlsx
+++ b/src/data/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\DABAD\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC0E2BF-BD1B-4D63-A6B9-71C33CD0DB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F5108C-41A7-41D5-BF84-1658C95B0042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2625" uniqueCount="752">
   <si>
     <t>Title</t>
   </si>
@@ -2248,6 +2248,42 @@
   </si>
   <si>
     <t>Ben Affleck</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>The Reader</t>
+  </si>
+  <si>
+    <t>Stephen Daldry</t>
+  </si>
+  <si>
+    <t>National Theatre Live: Prima Facie</t>
+  </si>
+  <si>
+    <t>Justin Martin</t>
+  </si>
+  <si>
+    <t>Succession [Season 1]</t>
+  </si>
+  <si>
+    <t>Jesse Armstrong</t>
+  </si>
+  <si>
+    <t>Succession [Season 2], Succession [Season 3], Succession [Season 4]</t>
+  </si>
+  <si>
+    <t>Sharp Objects</t>
+  </si>
+  <si>
+    <t>Marti Noxon</t>
+  </si>
+  <si>
+    <t>The End We Start From</t>
+  </si>
+  <si>
+    <t>Mahalia Belo</t>
   </si>
 </sst>
 </file>
@@ -2291,7 +2327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2327,6 +2363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2641,11 +2678,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P370"/>
+  <dimension ref="A1:P375"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <pane ySplit="1" topLeftCell="A364" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A375" sqref="A375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13551,6 +13588,143 @@
         <v>104</v>
       </c>
     </row>
+    <row r="371" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A371" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="B371" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C371" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="D371" s="3">
+        <v>2008</v>
+      </c>
+      <c r="E371" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="F371" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G371" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="K371" s="6">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="372" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A372" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B372" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C372" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="D372" s="3">
+        <v>2022</v>
+      </c>
+      <c r="E372" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="F372" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G372" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="K372" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="373" spans="1:11" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A373" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="B373" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C373" s="13" t="s">
+        <v>745</v>
+      </c>
+      <c r="D373" s="11">
+        <v>2018</v>
+      </c>
+      <c r="E373" s="12" t="s">
+        <v>746</v>
+      </c>
+      <c r="F373" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="G373" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="H373" s="12"/>
+      <c r="I373" s="12" t="s">
+        <v>747</v>
+      </c>
+      <c r="J373" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="K373" s="12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="374" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A374" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B374" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C374" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="D374" s="3">
+        <v>2018</v>
+      </c>
+      <c r="E374" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="F374" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="G374" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="K374" s="6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="375" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A375" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B375" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="D375" s="3">
+        <v>2023</v>
+      </c>
+      <c r="E375" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="F375" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="G375" s="6" t="s">
+        <v>419</v>
+      </c>
+      <c r="K375" s="6">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:P370" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P370">

</xml_diff>